<commit_message>
start of center bearing calculation
</commit_message>
<xml_diff>
--- a/documents/calculations/Spin Launch - Master Calculations.xlsx
+++ b/documents/calculations/Spin Launch - Master Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Spin Launch\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\projects\jm-space\open_spin_lauch\documents\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4A6F3A-D2B7-4E59-92A6-D471854A2D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BC5759-A3F4-42A1-9C9D-9547EB764D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{702068C3-7A62-4CAD-8ED5-C8846BDEF959}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" xr2:uid="{702068C3-7A62-4CAD-8ED5-C8846BDEF959}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="4" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="168">
   <si>
     <t>h_max [m]</t>
   </si>
@@ -503,6 +503,78 @@
   <si>
     <t>F_A_cw [N]</t>
   </si>
+  <si>
+    <t>Dimensioning Bearing</t>
+  </si>
+  <si>
+    <t>Driving radius</t>
+  </si>
+  <si>
+    <t>r_drive [m]</t>
+  </si>
+  <si>
+    <t>F_cr [N]</t>
+  </si>
+  <si>
+    <t>F_drive [N]</t>
+  </si>
+  <si>
+    <t>Centrifugal forces (oscillating)</t>
+  </si>
+  <si>
+    <t>Driving force through chain / crank handle (mostly static)</t>
+  </si>
+  <si>
+    <t>Approximate gravitational force (static)</t>
+  </si>
+  <si>
+    <t>F_grav [N]</t>
+  </si>
+  <si>
+    <t>Applied forces</t>
+  </si>
+  <si>
+    <t>Center motorization &amp; bearing</t>
+  </si>
+  <si>
+    <t>Outer radius of bearing</t>
+  </si>
+  <si>
+    <t>Inner radius of bearing</t>
+  </si>
+  <si>
+    <t>outer radius of inner ring</t>
+  </si>
+  <si>
+    <t>D_bear [mm]</t>
+  </si>
+  <si>
+    <t>d_bear [mm]</t>
+  </si>
+  <si>
+    <t>d1_bear [mm]</t>
+  </si>
+  <si>
+    <t>The projected area in Y (radial)</t>
+  </si>
+  <si>
+    <t>The projected area in X (axial)</t>
+  </si>
+  <si>
+    <t>w_bear [mm]</t>
+  </si>
+  <si>
+    <t>bearing width</t>
+  </si>
+  <si>
+    <t>A_projy [mm²]</t>
+  </si>
+  <si>
+    <t>A_projx [mm²]</t>
+  </si>
+  <si>
+    <t>Areas &amp; tensions</t>
+  </si>
 </sst>
 </file>
 
@@ -611,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -644,6 +716,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5969,10 +6050,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.749992370372631"/>
   </sheetPr>
-  <dimension ref="A1:K114"/>
+  <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="97" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I99" sqref="I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6207,7 +6288,7 @@
         <v>103</v>
       </c>
       <c r="D22" s="15">
-        <f>B70</f>
+        <f>B75</f>
         <v>2.6631421370738919</v>
       </c>
       <c r="E22" t="s">
@@ -6225,7 +6306,7 @@
         <v>93</v>
       </c>
       <c r="D23" s="15">
-        <f>B79</f>
+        <f>B84</f>
         <v>3.4706099103937511</v>
       </c>
       <c r="E23" t="s">
@@ -6243,7 +6324,7 @@
         <v>100</v>
       </c>
       <c r="D24" s="15">
-        <f>B83</f>
+        <f>B88</f>
         <v>1.6763767352014967</v>
       </c>
       <c r="E24" t="s">
@@ -6261,7 +6342,7 @@
         <v>96</v>
       </c>
       <c r="D25" s="15">
-        <f>B87</f>
+        <f>B92</f>
         <v>6.5747795014455406</v>
       </c>
       <c r="E25" t="s">
@@ -6273,7 +6354,7 @@
         <v>72</v>
       </c>
       <c r="D26" s="15">
-        <f>B88</f>
+        <f>B93</f>
         <v>91.257813264776885</v>
       </c>
       <c r="E26" t="s">
@@ -6296,7 +6377,7 @@
         <v>138</v>
       </c>
       <c r="D29" s="15">
-        <f>B97</f>
+        <f>B102</f>
         <v>2.6631421370738919</v>
       </c>
       <c r="E29" t="s">
@@ -6314,7 +6395,7 @@
         <v>139</v>
       </c>
       <c r="D30" s="15">
-        <f>B105</f>
+        <f>B110</f>
         <v>1.3875300569464575</v>
       </c>
       <c r="E30" t="s">
@@ -6332,7 +6413,7 @@
         <v>140</v>
       </c>
       <c r="D31" s="15">
-        <f>B109</f>
+        <f>B114</f>
         <v>0.70183645288697316</v>
       </c>
       <c r="E31" t="s">
@@ -6350,7 +6431,7 @@
         <v>141</v>
       </c>
       <c r="D32" s="15">
-        <f>B113</f>
+        <f>B118</f>
         <v>3.5872057397155261</v>
       </c>
       <c r="E32" t="s">
@@ -6362,587 +6443,732 @@
         <v>72</v>
       </c>
       <c r="D33" s="15">
-        <f>B114</f>
+        <f>B119</f>
         <v>167.26110614652993</v>
       </c>
       <c r="E33" t="s">
         <v>77</v>
       </c>
     </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" s="27"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>145</v>
+      </c>
+    </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B38" s="28">
+        <v>80</v>
+      </c>
+      <c r="C38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B39" s="28">
+        <v>50</v>
+      </c>
+      <c r="C39" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" s="28">
+        <v>58</v>
+      </c>
+      <c r="C40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" s="28">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="8" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="9" cm="1">
-        <f t="array" ref="B40">_xlfn.XLOOKUP(B25,Table1[[#All],[Material]],Table1[[#All],[Material Density '[kg/m^3']]])</f>
+      <c r="B45" s="9" cm="1">
+        <f t="array" ref="B45">_xlfn.XLOOKUP(B25,Table1[[#All],[Material]],Table1[[#All],[Material Density '[kg/m^3']]])</f>
         <v>1500</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B46" s="11">
         <f>(B23^2-B24^2)*PI()/4</f>
         <v>176.71458676442586</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="11">
-        <f>B41*B22*1000</f>
+      <c r="B47" s="11">
+        <f>B46*B22*1000</f>
         <v>353429.17352885171</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="14">
-        <f>(B42/10^9)*B40</f>
+      <c r="B48" s="14">
+        <f>(B47/10^9)*B45</f>
         <v>0.53014376029327759</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="4" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="11">
+      <c r="B49" s="11">
         <f>(B23^4-B24^4)*PI()/64</f>
         <v>11320.778214596032</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="8" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="9" cm="1">
-        <f t="array" ref="B47">_xlfn.XLOOKUP(B32,Table1[[#All],[Material]],Table1[[#All],[Material Density '[kg/m^3']]])</f>
+      <c r="B52" s="9" cm="1">
+        <f t="array" ref="B52">_xlfn.XLOOKUP(B32,Table1[[#All],[Material]],Table1[[#All],[Material Density '[kg/m^3']]])</f>
         <v>1500</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="4" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="11">
+      <c r="B53" s="11">
         <f>(B30^2-B31^2)*PI()/4</f>
         <v>176.71458676442586</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="4" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B49" s="11">
-        <f>B48*B29*1000</f>
+      <c r="B54" s="11">
+        <f>B53*B29*1000</f>
         <v>353429.17352885171</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="4" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="14">
-        <f>(B49/10^9)*B47</f>
+      <c r="B55" s="14">
+        <f>(B54/10^9)*B52</f>
         <v>0.53014376029327759</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="4" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B56" s="11">
         <f>(B30^4-B31^4)*PI()/64</f>
         <v>11320.778214596032</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>46</v>
       </c>
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="4" t="s">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B59" s="3">
         <f>(B22/B29)*B12</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="4" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B62" s="3">
         <f>B12*B22^2</f>
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="4" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B58" s="3">
-        <f>B54*B29^2</f>
+      <c r="B63" s="3">
+        <f>B59*B29^2</f>
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="4" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B59" s="3">
-        <f>(B43*B22^2)/3</f>
+      <c r="B64" s="3">
+        <f>(B48*B22^2)/3</f>
         <v>0.70685834705770345</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="4" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B60" s="3">
-        <f>(B50*B29^2)/3</f>
+      <c r="B65" s="3">
+        <f>(B55*B29^2)/3</f>
         <v>0.70685834705770345</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="4" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B61" s="3">
-        <f>B57+B58+B59+B60</f>
+      <c r="B66" s="3">
+        <f>B62+B63+B64+B65</f>
         <v>13.413716694115408</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="58" x14ac:dyDescent="0.35">
-      <c r="A65" s="4" t="s">
+    <row r="70" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A70" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B65" s="10">
+      <c r="B70" s="10">
         <f>(Kinematics!B14^2)/Main!B22</f>
         <v>266.62713713893902</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C70" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="4" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B66" s="10">
+      <c r="B71" s="10">
         <f>(Kinematics!B14^2)/(2*Main!B22)</f>
         <v>133.31356856946951</v>
       </c>
-      <c r="C66" s="7"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="4" t="s">
+      <c r="C71" s="7"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B67" s="10">
-        <f>B65*B12</f>
+      <c r="B72" s="10">
+        <f>B70*B12</f>
         <v>399.94070570840853</v>
       </c>
-      <c r="C67" s="7"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="4" t="s">
+      <c r="C72" s="7"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B68" s="10">
-        <f>B66*B43</f>
+      <c r="B73" s="10">
+        <f>B71*B48</f>
         <v>70.675356539534263</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="4" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B69" s="10">
-        <f>B67+B68</f>
+      <c r="B74" s="10">
+        <f>B72+B73</f>
         <v>470.61606224794281</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="4" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B70" s="12">
-        <f>B69/B41</f>
+      <c r="B75" s="12">
+        <f>B74/B46</f>
         <v>2.6631421370738919</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="9" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B73" s="16">
+      <c r="B78" s="16">
         <f>Kinetics!B14</f>
         <v>0.38487165042311255</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="9" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B74" s="23">
+      <c r="B79" s="23">
         <f>Kinetics!B19</f>
         <v>0.94328340096680074</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="4" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B75" s="3">
-        <f>B73*B12</f>
+      <c r="B80" s="3">
+        <f>B78*B12</f>
         <v>0.57730747563466878</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="4" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B76" s="13">
-        <f>(B73/2)*B43</f>
+      <c r="B81" s="13">
+        <f>(B78/2)*B48</f>
         <v>0.10201865199279435</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="4" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B77" s="3">
-        <f>B75+B76+B74</f>
+      <c r="B82" s="3">
+        <f>B80+B81+B79</f>
         <v>1.6226095285942639</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C82" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="4" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B78" s="3">
-        <f>B75*B22+B76*(B22/2)+B74*B22</f>
+      <c r="B83" s="3">
+        <f>B80*B22+B81*(B22/2)+B79*B22</f>
         <v>3.1432004051957332</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C83" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="4" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B79" s="13">
-        <f>(B78*1000)*B23/(2*B44)</f>
+      <c r="B84" s="13">
+        <f>(B83*1000)*B23/(2*B49)</f>
         <v>3.4706099103937511</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C84" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="9" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B82" s="15" cm="1">
-        <f t="array" ref="B82">_xlfn.XLOOKUP(B25,Table1[[#All],[Material]],Table1[[#All],[Elastic Modulus '[Mpa']]])</f>
+      <c r="B87" s="15" cm="1">
+        <f t="array" ref="B87">_xlfn.XLOOKUP(B25,Table1[[#All],[Material]],Table1[[#All],[Elastic Modulus '[Mpa']]])</f>
         <v>228000</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="6" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B83" s="3">
-        <f>B77*(B22*1000)^3/(3*B82*B44)</f>
+      <c r="B88" s="3">
+        <f>B82*(B22*1000)^3/(3*B87*B49)</f>
         <v>1.6763767352014967</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="9" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B86" s="15" cm="1">
-        <f t="array" ref="B86">_xlfn.XLOOKUP(B25,Table1[[#All],[Material]],Table1[[#All],[Yield Strenght '[Mpa']]])</f>
+      <c r="B91" s="15" cm="1">
+        <f t="array" ref="B91">_xlfn.XLOOKUP(B25,Table1[[#All],[Material]],Table1[[#All],[Yield Strenght '[Mpa']]])</f>
         <v>600</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B87" s="12">
-        <f>SQRT(B70^2+3*B79^2)</f>
-        <v>6.5747795014455406</v>
-      </c>
-      <c r="C87" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B88" s="11">
-        <f>B86/B87</f>
-        <v>91.257813264776885</v>
-      </c>
-      <c r="C88" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="12">
+        <f>SQRT(B75^2+3*B84^2)</f>
+        <v>6.5747795014455406</v>
+      </c>
+      <c r="C92" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B93" s="11">
+        <f>B91/B92</f>
+        <v>91.257813264776885</v>
+      </c>
+      <c r="C93" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B92" s="10">
+      <c r="B97" s="10">
         <f>(Kinematics!B14^2)/Main!B22</f>
         <v>266.62713713893902</v>
       </c>
-      <c r="C92" s="7"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="4" t="s">
+      <c r="C97" s="7"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B93" s="10">
+      <c r="B98" s="10">
         <f>(Kinematics!B14^2)/(2*Main!B22)</f>
         <v>133.31356856946951</v>
       </c>
-      <c r="C93" s="7"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="4" t="s">
+      <c r="C98" s="7"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B94" s="10">
-        <f>B92*B54</f>
+      <c r="B99" s="10">
+        <f>B97*B59</f>
         <v>399.94070570840853</v>
       </c>
-      <c r="C94" s="7"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="4" t="s">
+      <c r="C99" s="7"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B95" s="10">
-        <f>B93*B50</f>
+      <c r="B100" s="10">
+        <f>B98*B55</f>
         <v>70.675356539534263</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="4" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B96" s="10">
-        <f>B94+B95</f>
+      <c r="B101" s="10">
+        <f>B99+B100</f>
         <v>470.61606224794281</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="4" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B97" s="12">
-        <f>B96/B48</f>
+      <c r="B102" s="12">
+        <f>B101/B53</f>
         <v>2.6631421370738919</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" s="9" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B100" s="16">
+      <c r="B105" s="16">
         <f>Kinetics!B14</f>
         <v>0.38487165042311255</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="4" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B101" s="3">
-        <f>B100*B54</f>
+      <c r="B106" s="3">
+        <f>B105*B59</f>
         <v>0.57730747563466878</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="4" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B102" s="13">
-        <f>(B100/2)*B50</f>
+      <c r="B107" s="13">
+        <f>(B105/2)*B55</f>
         <v>0.10201865199279435</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="4" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B103" s="3">
-        <f>B101+B102</f>
+      <c r="B108" s="3">
+        <f>B106+B107</f>
         <v>0.67932612762746314</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C108" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="4" t="s">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B104" s="3">
-        <f>B101*B29+B102*(B29/2)</f>
+      <c r="B109" s="3">
+        <f>B106*B29+B107*(B29/2)</f>
         <v>1.2566336032621319</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C109" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="4" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B105" s="13">
-        <f>(B104*1000)*B30/(2*B51)</f>
+      <c r="B110" s="13">
+        <f>(B109*1000)*B30/(2*B56)</f>
         <v>1.3875300569464575</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C110" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="9" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B108" s="15" cm="1">
-        <f t="array" ref="B108">_xlfn.XLOOKUP(B32,Table1[[#All],[Material]],Table1[[#All],[Elastic Modulus '[Mpa']]])</f>
+      <c r="B113" s="15" cm="1">
+        <f t="array" ref="B113">_xlfn.XLOOKUP(B32,Table1[[#All],[Material]],Table1[[#All],[Elastic Modulus '[Mpa']]])</f>
         <v>228000</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="6" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B109" s="3">
-        <f>B103*(B29*1000)^3/(3*B108*B51)</f>
+      <c r="B114" s="3">
+        <f>B108*(B29*1000)^3/(3*B113*B56)</f>
         <v>0.70183645288697316</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" s="9" t="s">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B112" s="15" cm="1">
-        <f t="array" ref="B112">_xlfn.XLOOKUP(B32,Table1[[#All],[Material]],Table1[[#All],[Yield Strenght '[Mpa']]])</f>
+      <c r="B117" s="15" cm="1">
+        <f t="array" ref="B117">_xlfn.XLOOKUP(B32,Table1[[#All],[Material]],Table1[[#All],[Yield Strenght '[Mpa']]])</f>
         <v>600</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" s="4" t="s">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B113" s="12">
-        <f>SQRT(B97^2+3*B105^2)</f>
+      <c r="B118" s="12">
+        <f>SQRT(B102^2+3*B110^2)</f>
         <v>3.5872057397155261</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C118" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="4" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B114" s="11">
-        <f>B112/B113</f>
+      <c r="B119" s="11">
+        <f>B117/B118</f>
         <v>167.26110614652993</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C119" t="s">
         <v>77</v>
       </c>
     </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="B121" s="27"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B122" s="27"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B123" s="10">
+        <f>B99</f>
+        <v>399.94070570840853</v>
+      </c>
+      <c r="C123" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B124" s="10">
+        <f>D13/B37</f>
+        <v>44.678464431197291</v>
+      </c>
+      <c r="C124" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B125" s="10">
+        <f>(B12+B59+B48+B55) * 9.81</f>
+        <v>39.831420576954109</v>
+      </c>
+      <c r="C125" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="B127" s="25"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="B128" s="10">
+        <f>B38*B41</f>
+        <v>1600</v>
+      </c>
+      <c r="C128" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="B129" s="10">
+        <f>PI() /4 *(B40*B40 - B39*B39)</f>
+        <v>678.58401317539528</v>
+      </c>
+      <c r="C129" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A127:B127"/>
+  </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25 B32" xr:uid="{5BA042D7-8F26-4B17-8025-6A73066270B5}">
       <formula1>Material</formula1>
@@ -6960,8 +7186,8 @@
   </sheetPr>
   <dimension ref="A1:K1581"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B22" sqref="A22:B22"/>
+    <sheetView zoomScale="97" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27647,10 +27873,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView zoomScale="113" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27716,7 +27942,7 @@
         <v>89</v>
       </c>
       <c r="B12" s="9">
-        <f>Main!B61</f>
+        <f>Main!B66</f>
         <v>13.413716694115408</v>
       </c>
     </row>
@@ -27826,6 +28052,10 @@
       <c r="C25" t="s">
         <v>34</v>
       </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27839,7 +28069,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -27952,7 +28182,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="136" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>